<commit_message>
estimate_rt함수 추가 learnig decay 관련 수정 (target_rt 지정)
</commit_message>
<xml_diff>
--- a/DeepLearning/excel_output.xlsx
+++ b/DeepLearning/excel_output.xlsx
@@ -505,37 +505,37 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D2" t="n">
-        <v>1.83</v>
+        <v>1.082</v>
       </c>
       <c r="E2" t="n">
-        <v>2.844</v>
+        <v>4.098</v>
       </c>
       <c r="F2" t="n">
-        <v>2.328</v>
+        <v>1.404</v>
       </c>
       <c r="G2" t="n">
-        <v>2.37</v>
+        <v>24.492</v>
       </c>
       <c r="H2" t="n">
         <v>5.945647353655659e-05</v>
       </c>
       <c r="I2" t="n">
-        <v>5.782178609372769e-05</v>
+        <v>2.965634507584613e-05</v>
       </c>
       <c r="J2" t="n">
         <v>-42.25774765014648</v>
       </c>
       <c r="K2" t="n">
-        <v>-42.3788338485252</v>
+        <v>-45.27869493799358</v>
       </c>
       <c r="L2" t="n">
         <v>-6.098693013191223</v>
       </c>
       <c r="M2" t="n">
-        <v>-6.248993693212056</v>
+        <v>-9.623577012633623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>